<commit_message>
add expectation to mt
</commit_message>
<xml_diff>
--- a/adhafera/test/module_spec.xlsx
+++ b/adhafera/test/module_spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15960" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="110">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -1005,6 +1005,99 @@
     </rPh>
     <rPh sb="2" eb="4">
       <t>フセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>trueを返す</t>
+    <rPh sb="5" eb="6">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>登録した家計簿を返す</t>
+    <rPh sb="0" eb="2">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="4" eb="7">
+      <t>カケイボ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>正しい検索結果を返す</t>
+    <rPh sb="0" eb="1">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="3" eb="7">
+      <t>ケンサクケッカ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>全レコードを返す</t>
+    <rPh sb="0" eb="1">
+      <t>ゼン</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>更新されたレコードを返す</t>
+    <rPh sb="0" eb="2">
+      <t>コウシン</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>何も返さない</t>
+    <rPh sb="0" eb="1">
+      <t>ナニ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>正しい計算結果を返す</t>
+    <rPh sb="0" eb="1">
+      <t>タダ</t>
+    </rPh>
+    <rPh sb="3" eb="7">
+      <t>ケイサンケッカ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>falseを返す</t>
+    <rPh sb="6" eb="7">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>例外を返す</t>
+    <rPh sb="0" eb="2">
+      <t>レイガイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>カエ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1443,8 +1536,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="127">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1635,7 +1730,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="127">
+  <cellStyles count="129">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="5" builtinId="8" hidden="1"/>
@@ -1699,6 +1794,7 @@
     <cellStyle name="ハイパーリンク" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="123" builtinId="8" hidden="1"/>
     <cellStyle name="ハイパーリンク" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="ハイパーリンク" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="4" builtinId="9" hidden="1"/>
@@ -1763,6 +1859,7 @@
     <cellStyle name="表示済みのハイパーリンク" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="124" builtinId="9" hidden="1"/>
     <cellStyle name="表示済みのハイパーリンク" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="128" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2093,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2134,7 +2231,9 @@
       <c r="E3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="12">
@@ -2149,7 +2248,9 @@
       <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="12">
@@ -2164,7 +2265,9 @@
       <c r="E5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="12">
@@ -2179,7 +2282,9 @@
       <c r="E6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="12">
@@ -2194,7 +2299,9 @@
       <c r="E7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="12">
@@ -2209,7 +2316,9 @@
       <c r="E8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="12">
@@ -2224,7 +2333,9 @@
       <c r="E9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="12">
@@ -2239,7 +2350,9 @@
       <c r="E10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="12">
@@ -2254,7 +2367,9 @@
       <c r="E11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="12">
@@ -2269,7 +2384,9 @@
       <c r="E12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="12">
@@ -2284,7 +2401,9 @@
       <c r="E13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="12">
@@ -2299,7 +2418,9 @@
       <c r="E14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="12">
@@ -2314,7 +2435,9 @@
       <c r="E15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="12">
@@ -2329,7 +2452,9 @@
       <c r="E16" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="11"/>
+      <c r="F16" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="12">
@@ -2344,7 +2469,9 @@
       <c r="E17" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="12">
@@ -2359,7 +2486,9 @@
       <c r="E18" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="12">
@@ -2374,7 +2503,9 @@
       <c r="E19" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="12">
@@ -2389,7 +2520,9 @@
       <c r="E20" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="14"/>
+      <c r="F20" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="12">
@@ -2404,7 +2537,9 @@
       <c r="E21" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="12">
@@ -2419,7 +2554,9 @@
       <c r="E22" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="12">
@@ -2434,7 +2571,9 @@
       <c r="E23" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="12">
@@ -2449,7 +2588,9 @@
       <c r="E24" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" s="12">
@@ -2464,7 +2605,9 @@
       <c r="E25" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="14"/>
+      <c r="F25" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="12">
@@ -2479,7 +2622,9 @@
       <c r="E26" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="12">
@@ -2494,7 +2639,9 @@
       <c r="E27" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="12">
@@ -2509,7 +2656,9 @@
       <c r="E28" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="22">
@@ -2524,7 +2673,9 @@
       <c r="E29" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="11"/>
+      <c r="F29" s="11" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="12">
@@ -2539,7 +2690,9 @@
       <c r="E30" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F30" s="14"/>
+      <c r="F30" s="14" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="22">
@@ -2554,7 +2707,9 @@
       <c r="E31" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="14"/>
+      <c r="F31" s="14" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="12">
@@ -2569,7 +2724,9 @@
       <c r="E32" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="F32" s="14" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="22">
@@ -2584,7 +2741,9 @@
       <c r="E33" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="14"/>
+      <c r="F33" s="14" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="12">
@@ -2599,7 +2758,9 @@
       <c r="E34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="14" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="22">
@@ -2614,7 +2775,9 @@
       <c r="E35" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" s="12">
@@ -2629,7 +2792,9 @@
       <c r="E36" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F36" s="14"/>
+      <c r="F36" s="14" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" s="22">
@@ -2644,7 +2809,9 @@
       <c r="E37" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F37" s="14"/>
+      <c r="F37" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" s="12">
@@ -2659,7 +2826,9 @@
       <c r="E38" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F38" s="14"/>
+      <c r="F38" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39" s="22">
@@ -2674,7 +2843,9 @@
       <c r="E39" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="F39" s="14"/>
+      <c r="F39" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="40" spans="2:6">
       <c r="B40" s="12">
@@ -2689,7 +2860,9 @@
       <c r="E40" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F40" s="14"/>
+      <c r="F40" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="41" spans="2:6">
       <c r="B41" s="22">
@@ -2704,7 +2877,9 @@
       <c r="E41" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="F41" s="14"/>
+      <c r="F41" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="42" spans="2:6">
       <c r="B42" s="12">
@@ -2719,7 +2894,9 @@
       <c r="E42" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="14"/>
+      <c r="F42" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="43" spans="2:6">
       <c r="B43" s="22">
@@ -2734,7 +2911,9 @@
       <c r="E43" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="F43" s="14"/>
+      <c r="F43" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" s="12">
@@ -2749,7 +2928,9 @@
       <c r="E44" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F44" s="14"/>
+      <c r="F44" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="22">
@@ -2764,7 +2945,9 @@
       <c r="E45" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F45" s="14"/>
+      <c r="F45" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46" s="12">
@@ -2779,7 +2962,9 @@
       <c r="E46" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F46" s="14"/>
+      <c r="F46" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="47" spans="2:6">
       <c r="B47" s="22">
@@ -2794,7 +2979,9 @@
       <c r="E47" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F47" s="14"/>
+      <c r="F47" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="48" spans="2:6">
       <c r="B48" s="12">
@@ -2809,7 +2996,9 @@
       <c r="E48" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="F48" s="14"/>
+      <c r="F48" s="14" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="49" spans="2:6">
       <c r="B49" s="22">
@@ -2824,7 +3013,9 @@
       <c r="E49" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F49" s="14"/>
+      <c r="F49" s="14" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="50" spans="2:6">
       <c r="B50" s="12">
@@ -2839,7 +3030,9 @@
       <c r="E50" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F50" s="14"/>
+      <c r="F50" s="14" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="22">
@@ -2854,7 +3047,9 @@
       <c r="E51" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F51" s="14"/>
+      <c r="F51" s="14" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="52" spans="2:6">
       <c r="B52" s="12">
@@ -2869,7 +3064,9 @@
       <c r="E52" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="F52" s="14"/>
+      <c r="F52" s="14" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53" s="22">
@@ -2884,7 +3081,9 @@
       <c r="E53" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="F53" s="14"/>
+      <c r="F53" s="14" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54" s="12">
@@ -2899,7 +3098,9 @@
       <c r="E54" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F54" s="29"/>
+      <c r="F54" s="29" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="55" spans="2:6">
       <c r="B55" s="22">
@@ -2914,7 +3115,9 @@
       <c r="E55" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F55" s="29"/>
+      <c r="F55" s="29" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="56" spans="2:6" ht="19" thickBot="1">
       <c r="B56" s="30">
@@ -2929,7 +3132,9 @@
       <c r="E56" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="F56" s="26"/>
+      <c r="F56" s="26" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2947,8 +3152,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2988,7 +3193,9 @@
       <c r="E3" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="32">
@@ -3003,7 +3210,9 @@
       <c r="E4" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="32">
@@ -3018,7 +3227,9 @@
       <c r="E5" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="14"/>
+      <c r="F5" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="32">
@@ -3033,7 +3244,9 @@
       <c r="E6" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="14"/>
+      <c r="F6" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="32">
@@ -3048,7 +3261,9 @@
       <c r="E7" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="14"/>
+      <c r="F7" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="32">
@@ -3063,7 +3278,9 @@
       <c r="E8" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="14"/>
+      <c r="F8" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="32">
@@ -3078,7 +3295,9 @@
       <c r="E9" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F9" s="14"/>
+      <c r="F9" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="32">
@@ -3093,7 +3312,9 @@
       <c r="E10" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="14"/>
+      <c r="F10" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="32">
@@ -3108,7 +3329,9 @@
       <c r="E11" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="32">
@@ -3123,7 +3346,9 @@
       <c r="E12" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="32">
@@ -3138,7 +3363,9 @@
       <c r="E13" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="14"/>
+      <c r="F13" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="32">
@@ -3153,7 +3380,9 @@
       <c r="E14" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="32">
@@ -3168,7 +3397,9 @@
       <c r="E15" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F15" s="14"/>
+      <c r="F15" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="32">
@@ -3183,7 +3414,9 @@
       <c r="E16" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F16" s="14"/>
+      <c r="F16" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="32">
@@ -3198,7 +3431,9 @@
       <c r="E17" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="14"/>
+      <c r="F17" s="14" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="32">
@@ -3213,7 +3448,9 @@
       <c r="E18" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="14"/>
+      <c r="F18" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="32">
@@ -3228,7 +3465,9 @@
       <c r="E19" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="32">
@@ -3243,7 +3482,9 @@
       <c r="E20" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F20" s="14"/>
+      <c r="F20" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="32">
@@ -3258,7 +3499,9 @@
       <c r="E21" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="32">
@@ -3273,7 +3516,9 @@
       <c r="E22" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="14"/>
+      <c r="F22" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="32">
@@ -3288,7 +3533,9 @@
       <c r="E23" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="14"/>
+      <c r="F23" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="32">
@@ -3303,7 +3550,9 @@
       <c r="E24" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F24" s="14"/>
+      <c r="F24" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" s="32">
@@ -3318,7 +3567,9 @@
       <c r="E25" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F25" s="14"/>
+      <c r="F25" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="32">
@@ -3333,7 +3584,9 @@
       <c r="E26" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="14"/>
+      <c r="F26" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="32">
@@ -3348,7 +3601,9 @@
       <c r="E27" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="32">
@@ -3363,7 +3618,9 @@
       <c r="E28" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="14"/>
+      <c r="F28" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" s="32">
@@ -3378,7 +3635,9 @@
       <c r="E29" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="F29" s="14"/>
+      <c r="F29" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="32">
@@ -3393,7 +3652,9 @@
       <c r="E30" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="14"/>
+      <c r="F30" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="32">
@@ -3408,7 +3669,9 @@
       <c r="E31" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="14"/>
+      <c r="F31" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="32">
@@ -3423,7 +3686,9 @@
       <c r="E32" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F32" s="14"/>
+      <c r="F32" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="32">
@@ -3438,7 +3703,9 @@
       <c r="E33" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="F33" s="14"/>
+      <c r="F33" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="32">
@@ -3453,7 +3720,9 @@
       <c r="E34" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F34" s="14"/>
+      <c r="F34" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="32">
@@ -3468,7 +3737,9 @@
       <c r="E35" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" s="32">
@@ -3483,7 +3754,9 @@
       <c r="E36" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="F36" s="14"/>
+      <c r="F36" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="37" spans="2:6" ht="19" thickBot="1">
       <c r="B37" s="30">
@@ -3498,7 +3771,9 @@
       <c r="E37" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="F37" s="16"/>
+      <c r="F37" s="16" t="s">
+        <v>109</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
add module test case
</commit_message>
<xml_diff>
--- a/adhafera/test/module_spec.xlsx
+++ b/adhafera/test/module_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -48,10 +48,6 @@
     <t>1.0.0</t>
   </si>
   <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>条件</t>
     <rPh sb="0" eb="2">
       <t>ジョウケン</t>
@@ -59,26 +55,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>InputChecker.checkEmrpty</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>inputs:[]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>[0]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>InputChecker.checkDate</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -100,6 +80,204 @@
   </si>
   <si>
     <t>true</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.sendRequest</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs:[
+  '2015-01-01',
+  'テスト用データ',
+  'テスト',
+  '100',
+  'expense'
+]</t>
+    <rPh sb="31" eb="32">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 201,
+  body: {
+    account_type: 'expense',
+    date: '2015-01-01',
+    content: 'テスト用データ',
+    category: 'テスト',
+    price: 100
+  }
+}</t>
+    <rPh sb="97" eb="98">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs:[
+  '2015-01-01',
+  'テスト用データ',
+  'テスト',
+  '100',
+  'expense'
+]</t>
+    <rPh sb="31" eb="32">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>InputChecker.checkEmpty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[3]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[0,1,2,3,4]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>InputChecker.checkDate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Inputchecker.checkPrice</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>date: 'invalid_date'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>price: 'invalid_price'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '2015-01-01',
+  'テスト用データ',
+  null,
+  '100',
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HTTPClient.sendRequest</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '01-01-2015',
+  'テスト用データ',
+  'テスト',
+  '100',
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '2015-01-01',
+  null,
+  'テスト',
+  null,
+  'expense'
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 400,
+  body: {
+    [error_code: 'absent_param_category']
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 400,
+  body: {
+    [error_code: 'invalid_param_date']
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 400,
+  body: {
+    [
+      error_code: 'absent_param_content',
+      error_code: 'absent_param_price'
+    ]
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '01-01-2015',
+  'テスト用データ',
+  'テスト',
+  '-100',
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>{
+  status: 400,
+  body: {
+    [
+      error_code: 'invalid_param_date',
+      error_code: 'invalid_param_price'
+    ]
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [
+  '2015-01-01',
+  'テスト用データ',
+  'テスト',
+  null,
+  'expense'
+]</t>
+    <rPh sb="32" eb="33">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>inputs: [null, null, null, null, null]</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -156,7 +334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -281,43 +459,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -430,32 +571,12 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -652,19 +773,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -677,53 +798,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="191">
@@ -1246,9 +1349,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G30"/>
+  <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="47.1640625" customWidth="1"/>
+    <col min="5" max="5" width="37.83203125" customWidth="1"/>
+    <col min="6" max="7" width="47.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="19" thickBot="1"/>
+    <row r="2" spans="2:7" ht="19" thickBot="1">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="96">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="136" thickBot="1">
+      <c r="B6" s="14">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:G10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1275,642 +1499,155 @@
         <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="8">
+    <row r="3" spans="2:7" ht="96">
+      <c r="B3" s="15">
         <v>1</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="13" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="8">
+      <c r="B4" s="15">
         <v>2</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="27" t="s">
-        <v>17</v>
+      <c r="G4" s="13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="8">
+      <c r="B5" s="15">
         <v>3</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="27" t="s">
-        <v>18</v>
+      <c r="G5" s="16" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="8">
-        <v>4</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
-    </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="8">
-        <v>5</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
-    </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="8">
-        <v>6</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="8">
-        <v>7</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
-    </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="8">
-        <v>8</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="8">
-        <v>9</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="8">
-        <v>10</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="8">
-        <v>11</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="8">
-        <v>12</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="8">
-        <v>13</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="8">
-        <v>14</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="8">
-        <v>15</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="8">
-        <v>16</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="8">
-        <v>17</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="8">
-        <v>18</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="8">
-        <v>19</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="13"/>
-    </row>
-    <row r="22" spans="2:7">
-      <c r="B22" s="8">
-        <v>20</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="13"/>
-    </row>
-    <row r="23" spans="2:7">
-      <c r="B23" s="8">
-        <v>21</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" spans="2:7">
-      <c r="B24" s="8">
-        <v>22</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="8">
-        <v>23</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="8">
-        <v>24</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="13"/>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="8">
-        <v>25</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="13"/>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="8">
-        <v>26</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="10"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="13"/>
-    </row>
-    <row r="29" spans="2:7">
-      <c r="B29" s="8">
-        <v>27</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="10"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="13"/>
-    </row>
-    <row r="30" spans="2:7" ht="19" thickBot="1">
-      <c r="B30" s="15">
-        <v>28</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="16"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="19"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="3.1640625" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" customWidth="1"/>
-    <col min="5" max="5" width="37.83203125" customWidth="1"/>
-    <col min="6" max="7" width="47.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="19" thickBot="1"/>
-    <row r="2" spans="2:7" ht="19" thickBot="1">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7">
-      <c r="B3" s="20">
-        <v>1</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="2:7">
-      <c r="B4" s="20">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
-    </row>
-    <row r="5" spans="2:7">
-      <c r="B5" s="20">
-        <v>3</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="2:7">
-      <c r="B6" s="20">
+      <c r="B6" s="15">
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
+      <c r="D6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="2:7">
-      <c r="B7" s="20">
+    <row r="7" spans="2:7" ht="96">
+      <c r="B7" s="15">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
+      <c r="D7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>28</v>
+      </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="21" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="8" spans="2:7">
-      <c r="B8" s="20">
+    <row r="8" spans="2:7" ht="96">
+      <c r="B8" s="15">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
+      <c r="D8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="21" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="9" spans="2:7">
-      <c r="B9" s="20">
+    <row r="9" spans="2:7" ht="122">
+      <c r="B9" s="15">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="11"/>
+      <c r="D9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>31</v>
+      </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="21" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="10" spans="2:7">
-      <c r="B10" s="20">
+    <row r="10" spans="2:7" ht="123" thickBot="1">
+      <c r="B10" s="14">
         <v>8</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="20">
-        <v>9</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="20">
-        <v>10</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="20">
-        <v>11</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="2:7">
-      <c r="B14" s="20">
-        <v>12</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="20">
-        <v>13</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="2:7">
-      <c r="B16" s="20">
-        <v>14</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="20">
-        <v>15</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="2:7">
-      <c r="B18" s="20">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="2:7">
-      <c r="B19" s="20">
-        <v>17</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="13"/>
-    </row>
-    <row r="20" spans="2:7">
-      <c r="B20" s="20">
-        <v>18</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="26"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="13"/>
-    </row>
-    <row r="21" spans="2:7" ht="19" thickBot="1">
-      <c r="B21" s="15">
-        <v>19</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24"/>
+      <c r="D10" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="19"/>
+      <c r="G10" s="20" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>